<commit_message>
generated RDF/XML of trento
</commit_message>
<xml_diff>
--- a/source-data/dataTrento/servizionline.xlsx
+++ b/source-data/dataTrento/servizionline.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" firstSheet="3" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Public Service" sheetId="1" r:id="rId1"/>
@@ -4239,37 +4239,37 @@
   </sheetPr>
   <dimension ref="A1:Z60"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U52" sqref="U52"/>
+      <selection pane="bottomLeft" activeCell="S52" sqref="A52:S52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.1796875"/>
-    <col min="2" max="2" width="47.54296875"/>
-    <col min="3" max="3" width="101.54296875"/>
-    <col min="4" max="4" width="23.453125"/>
-    <col min="5" max="5" width="11.1796875"/>
-    <col min="6" max="6" width="22.26953125"/>
-    <col min="7" max="7" width="12.7265625"/>
-    <col min="8" max="8" width="11.1796875"/>
-    <col min="10" max="10" width="6.26953125"/>
-    <col min="11" max="11" width="13.1796875"/>
-    <col min="12" max="12" width="11.453125"/>
-    <col min="14" max="14" width="59.1796875"/>
-    <col min="15" max="15" width="15.81640625"/>
-    <col min="16" max="17" width="41.1796875"/>
-    <col min="18" max="18" width="30.453125"/>
+    <col min="1" max="1" width="19.140625"/>
+    <col min="2" max="2" width="47.5703125"/>
+    <col min="3" max="3" width="101.5703125"/>
+    <col min="4" max="4" width="23.42578125"/>
+    <col min="5" max="5" width="11.140625"/>
+    <col min="6" max="6" width="22.28515625"/>
+    <col min="7" max="7" width="12.7109375"/>
+    <col min="8" max="8" width="11.140625"/>
+    <col min="10" max="10" width="6.28515625"/>
+    <col min="11" max="11" width="13.140625"/>
+    <col min="12" max="12" width="11.42578125"/>
+    <col min="14" max="14" width="59.140625"/>
+    <col min="15" max="15" width="15.85546875"/>
+    <col min="16" max="17" width="41.140625"/>
+    <col min="18" max="18" width="30.42578125"/>
     <col min="19" max="19" width="41"/>
-    <col min="20" max="20" width="6.81640625"/>
-    <col min="21" max="21" width="16.26953125"/>
-    <col min="22" max="22" width="55.453125"/>
-    <col min="23" max="23" width="15.26953125"/>
-    <col min="24" max="24" width="19.26953125"/>
-    <col min="25" max="25" width="13.1796875"/>
-    <col min="26" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="20" max="20" width="6.85546875"/>
+    <col min="21" max="21" width="16.28515625"/>
+    <col min="22" max="22" width="55.42578125"/>
+    <col min="23" max="23" width="15.28515625"/>
+    <col min="24" max="24" width="19.28515625"/>
+    <col min="25" max="25" width="13.140625"/>
+    <col min="26" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="25.5" customHeight="1">
@@ -4352,7 +4352,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="10" customFormat="1" ht="174">
+    <row r="2" spans="1:26" s="10" customFormat="1" ht="180">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -4420,7 +4420,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="126">
+    <row r="3" spans="1:26" ht="156.75">
       <c r="A3" s="11" t="s">
         <v>46</v>
       </c>
@@ -4490,7 +4490,7 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:26" ht="126">
+    <row r="4" spans="1:26" ht="156.75">
       <c r="A4" s="11" t="s">
         <v>63</v>
       </c>
@@ -4556,7 +4556,7 @@
       <c r="Y4" s="11"/>
       <c r="Z4" s="12"/>
     </row>
-    <row r="5" spans="1:26" ht="203">
+    <row r="5" spans="1:26" ht="210">
       <c r="A5" s="12" t="s">
         <v>79</v>
       </c>
@@ -4628,7 +4628,7 @@
       <c r="Y5" s="11"/>
       <c r="Z5" s="11"/>
     </row>
-    <row r="6" spans="1:26" ht="203">
+    <row r="6" spans="1:26" ht="210">
       <c r="A6" s="12" t="s">
         <v>90</v>
       </c>
@@ -4700,7 +4700,7 @@
       <c r="Y6" s="11"/>
       <c r="Z6" s="11"/>
     </row>
-    <row r="7" spans="1:26" ht="210">
+    <row r="7" spans="1:26" ht="213.75">
       <c r="A7" s="12" t="s">
         <v>99</v>
       </c>
@@ -4772,7 +4772,7 @@
       <c r="Y7" s="11"/>
       <c r="Z7" s="11"/>
     </row>
-    <row r="8" spans="1:26" ht="217.5">
+    <row r="8" spans="1:26" ht="225">
       <c r="A8" s="12" t="s">
         <v>105</v>
       </c>
@@ -4844,7 +4844,7 @@
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
     </row>
-    <row r="9" spans="1:26" ht="159.5">
+    <row r="9" spans="1:26" ht="195">
       <c r="A9" s="12" t="s">
         <v>113</v>
       </c>
@@ -4912,7 +4912,7 @@
       <c r="Y9" s="11"/>
       <c r="Z9" s="11"/>
     </row>
-    <row r="10" spans="1:26" ht="154">
+    <row r="10" spans="1:26" ht="156.75">
       <c r="A10" s="12" t="s">
         <v>127</v>
       </c>
@@ -4984,7 +4984,7 @@
       <c r="Y10" s="11"/>
       <c r="Z10" s="11"/>
     </row>
-    <row r="11" spans="1:26" ht="232">
+    <row r="11" spans="1:26" ht="240">
       <c r="A11" s="12" t="s">
         <v>139</v>
       </c>
@@ -5054,7 +5054,7 @@
       <c r="Y11" s="11"/>
       <c r="Z11" s="11"/>
     </row>
-    <row r="12" spans="1:26" ht="252">
+    <row r="12" spans="1:26" ht="256.5">
       <c r="A12" s="12" t="s">
         <v>150</v>
       </c>
@@ -5124,7 +5124,7 @@
       <c r="Y12" s="11"/>
       <c r="Z12" s="11"/>
     </row>
-    <row r="13" spans="1:26" ht="126">
+    <row r="13" spans="1:26" ht="156.75">
       <c r="A13" s="12" t="s">
         <v>156</v>
       </c>
@@ -5194,7 +5194,7 @@
       <c r="Y13" s="11"/>
       <c r="Z13" s="11"/>
     </row>
-    <row r="14" spans="1:26" ht="252">
+    <row r="14" spans="1:26" ht="256.5">
       <c r="A14" s="12" t="s">
         <v>167</v>
       </c>
@@ -5264,7 +5264,7 @@
       <c r="Y14" s="11"/>
       <c r="Z14" s="12"/>
     </row>
-    <row r="15" spans="1:26" ht="392">
+    <row r="15" spans="1:26" ht="409.5">
       <c r="A15" s="12" t="s">
         <v>182</v>
       </c>
@@ -5330,7 +5330,7 @@
       <c r="Y15" s="11"/>
       <c r="Z15" s="12"/>
     </row>
-    <row r="16" spans="1:26" ht="196">
+    <row r="16" spans="1:26" ht="213.75">
       <c r="A16" s="12" t="s">
         <v>192</v>
       </c>
@@ -5396,7 +5396,7 @@
       <c r="Y16" s="11"/>
       <c r="Z16" s="12"/>
     </row>
-    <row r="17" spans="1:26" ht="154">
+    <row r="17" spans="1:26" ht="171">
       <c r="A17" s="12" t="s">
         <v>203</v>
       </c>
@@ -5466,7 +5466,7 @@
       <c r="Y17" s="11"/>
       <c r="Z17" s="12"/>
     </row>
-    <row r="18" spans="1:26" ht="126">
+    <row r="18" spans="1:26" ht="156.75">
       <c r="A18" s="12" t="s">
         <v>210</v>
       </c>
@@ -5536,7 +5536,7 @@
       <c r="Y18" s="11"/>
       <c r="Z18" s="12"/>
     </row>
-    <row r="19" spans="1:26" ht="168">
+    <row r="19" spans="1:26" ht="171">
       <c r="A19" s="12" t="s">
         <v>223</v>
       </c>
@@ -5604,7 +5604,7 @@
       <c r="Y19" s="11"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="1:26" ht="168">
+    <row r="20" spans="1:26" ht="185.25">
       <c r="A20" s="12" t="s">
         <v>238</v>
       </c>
@@ -5674,7 +5674,7 @@
       <c r="Y20" s="11"/>
       <c r="Z20" s="12"/>
     </row>
-    <row r="21" spans="1:26" ht="252">
+    <row r="21" spans="1:26" ht="270.75">
       <c r="A21" s="12" t="s">
         <v>246</v>
       </c>
@@ -5736,7 +5736,7 @@
       <c r="Y21" s="11"/>
       <c r="Z21" s="12"/>
     </row>
-    <row r="22" spans="1:26" ht="126">
+    <row r="22" spans="1:26" ht="156.75">
       <c r="A22" s="12" t="s">
         <v>257</v>
       </c>
@@ -5796,7 +5796,7 @@
       <c r="Y22" s="11"/>
       <c r="Z22" s="12"/>
     </row>
-    <row r="23" spans="1:26" ht="126">
+    <row r="23" spans="1:26" ht="156.75">
       <c r="A23" s="12" t="s">
         <v>269</v>
       </c>
@@ -5856,7 +5856,7 @@
       <c r="Y23" s="11"/>
       <c r="Z23" s="20"/>
     </row>
-    <row r="24" spans="1:26" ht="126">
+    <row r="24" spans="1:26" ht="156.75">
       <c r="A24" s="12" t="s">
         <v>279</v>
       </c>
@@ -5920,7 +5920,7 @@
       <c r="Y24" s="11"/>
       <c r="Z24" s="12"/>
     </row>
-    <row r="25" spans="1:26" ht="168">
+    <row r="25" spans="1:26" ht="171">
       <c r="A25" s="12" t="s">
         <v>292</v>
       </c>
@@ -5984,7 +5984,7 @@
       <c r="Y25" s="11"/>
       <c r="Z25" s="12"/>
     </row>
-    <row r="26" spans="1:26" ht="182">
+    <row r="26" spans="1:26" ht="185.25">
       <c r="A26" s="12" t="s">
         <v>304</v>
       </c>
@@ -6050,7 +6050,7 @@
       <c r="Y26" s="11"/>
       <c r="Z26" s="12"/>
     </row>
-    <row r="27" spans="1:26" ht="126">
+    <row r="27" spans="1:26" ht="156.75">
       <c r="A27" s="12" t="s">
         <v>316</v>
       </c>
@@ -6116,7 +6116,7 @@
       <c r="Y27" s="11"/>
       <c r="Z27" s="20"/>
     </row>
-    <row r="28" spans="1:26" ht="126">
+    <row r="28" spans="1:26" ht="156.75">
       <c r="A28" s="12" t="s">
         <v>329</v>
       </c>
@@ -6184,7 +6184,7 @@
       <c r="Y28" s="11"/>
       <c r="Z28" s="12"/>
     </row>
-    <row r="29" spans="1:26" ht="168">
+    <row r="29" spans="1:26" ht="185.25">
       <c r="A29" s="12" t="s">
         <v>340</v>
       </c>
@@ -6246,7 +6246,7 @@
       <c r="Y29" s="11"/>
       <c r="Z29" s="12"/>
     </row>
-    <row r="30" spans="1:26" ht="168">
+    <row r="30" spans="1:26" ht="185.25">
       <c r="A30" s="12" t="s">
         <v>347</v>
       </c>
@@ -6306,7 +6306,7 @@
       <c r="Y30" s="11"/>
       <c r="Z30" s="12"/>
     </row>
-    <row r="31" spans="1:26" ht="246.5">
+    <row r="31" spans="1:26" ht="300">
       <c r="A31" s="12" t="s">
         <v>353</v>
       </c>
@@ -6370,7 +6370,7 @@
       <c r="Y31" s="11"/>
       <c r="Z31" s="20"/>
     </row>
-    <row r="32" spans="1:26" ht="168">
+    <row r="32" spans="1:26" ht="185.25">
       <c r="A32" s="12" t="s">
         <v>364</v>
       </c>
@@ -6436,7 +6436,7 @@
       <c r="Y32" s="11"/>
       <c r="Z32" s="12"/>
     </row>
-    <row r="33" spans="1:26" ht="126">
+    <row r="33" spans="1:26" ht="156.75">
       <c r="A33" s="12" t="s">
         <v>374</v>
       </c>
@@ -6500,7 +6500,7 @@
       <c r="Y33" s="11"/>
       <c r="Z33" s="12"/>
     </row>
-    <row r="34" spans="1:26" ht="168">
+    <row r="34" spans="1:26" ht="199.5">
       <c r="A34" s="12" t="s">
         <v>381</v>
       </c>
@@ -6564,7 +6564,7 @@
       <c r="Y34" s="11"/>
       <c r="Z34" s="20"/>
     </row>
-    <row r="35" spans="1:26" ht="168">
+    <row r="35" spans="1:26" ht="199.5">
       <c r="A35" s="12" t="s">
         <v>393</v>
       </c>
@@ -6628,7 +6628,7 @@
       <c r="Y35" s="11"/>
       <c r="Z35" s="20"/>
     </row>
-    <row r="36" spans="1:26" ht="168">
+    <row r="36" spans="1:26" ht="199.5">
       <c r="A36" s="12" t="s">
         <v>401</v>
       </c>
@@ -6692,7 +6692,7 @@
       <c r="Y36" s="11"/>
       <c r="Z36" s="20"/>
     </row>
-    <row r="37" spans="1:26" ht="126">
+    <row r="37" spans="1:26" ht="156.75">
       <c r="A37" s="12" t="s">
         <v>405</v>
       </c>
@@ -6762,7 +6762,7 @@
       <c r="Y37" s="11"/>
       <c r="Z37" s="12"/>
     </row>
-    <row r="38" spans="1:26" ht="126">
+    <row r="38" spans="1:26" ht="156.75">
       <c r="A38" s="12" t="s">
         <v>412</v>
       </c>
@@ -6828,7 +6828,7 @@
       <c r="Y38" s="11"/>
       <c r="Z38" s="12"/>
     </row>
-    <row r="39" spans="1:26" ht="159.5">
+    <row r="39" spans="1:26" ht="195">
       <c r="A39" s="12" t="s">
         <v>421</v>
       </c>
@@ -6892,7 +6892,7 @@
       <c r="Y39" s="11"/>
       <c r="Z39" s="12"/>
     </row>
-    <row r="40" spans="1:26" ht="159.5">
+    <row r="40" spans="1:26" ht="195">
       <c r="A40" s="21" t="s">
         <v>431</v>
       </c>
@@ -6956,7 +6956,7 @@
       <c r="Y40" s="11"/>
       <c r="Z40" s="20"/>
     </row>
-    <row r="41" spans="1:26" ht="126">
+    <row r="41" spans="1:26" ht="156.75">
       <c r="A41" s="22" t="s">
         <v>439</v>
       </c>
@@ -7018,7 +7018,7 @@
       <c r="Y41" s="22"/>
       <c r="Z41" s="22"/>
     </row>
-    <row r="42" spans="1:26" ht="168">
+    <row r="42" spans="1:26" ht="199.5">
       <c r="A42" s="21" t="s">
         <v>443</v>
       </c>
@@ -7082,7 +7082,7 @@
       <c r="Y42" s="11"/>
       <c r="Z42" s="12"/>
     </row>
-    <row r="43" spans="1:26" ht="126">
+    <row r="43" spans="1:26" ht="156.75">
       <c r="A43" s="21" t="s">
         <v>454</v>
       </c>
@@ -7142,7 +7142,7 @@
       <c r="Y43" s="11"/>
       <c r="Z43" s="12"/>
     </row>
-    <row r="44" spans="1:26" ht="126">
+    <row r="44" spans="1:26" ht="156.75">
       <c r="A44" s="21" t="s">
         <v>461</v>
       </c>
@@ -7202,7 +7202,7 @@
       <c r="Y44" s="11"/>
       <c r="Z44" s="12"/>
     </row>
-    <row r="45" spans="1:26" ht="126">
+    <row r="45" spans="1:26" ht="156.75">
       <c r="A45" s="21" t="s">
         <v>466</v>
       </c>
@@ -7262,7 +7262,7 @@
       <c r="Y45" s="11"/>
       <c r="Z45" s="12"/>
     </row>
-    <row r="46" spans="1:26" ht="168">
+    <row r="46" spans="1:26" ht="185.25">
       <c r="A46" s="21" t="s">
         <v>469</v>
       </c>
@@ -7320,7 +7320,7 @@
       <c r="Y46" s="11"/>
       <c r="Z46" s="20"/>
     </row>
-    <row r="47" spans="1:26" ht="126">
+    <row r="47" spans="1:26" ht="156.75">
       <c r="A47" s="21" t="s">
         <v>474</v>
       </c>
@@ -7382,7 +7382,7 @@
       <c r="Y47" s="11"/>
       <c r="Z47" s="12"/>
     </row>
-    <row r="48" spans="1:26" ht="126">
+    <row r="48" spans="1:26" ht="156.75">
       <c r="A48" s="21" t="s">
         <v>478</v>
       </c>
@@ -7444,7 +7444,7 @@
       <c r="Y48" s="11"/>
       <c r="Z48" s="20"/>
     </row>
-    <row r="49" spans="1:26" ht="168">
+    <row r="49" spans="1:26" ht="171">
       <c r="A49" s="21" t="s">
         <v>486</v>
       </c>
@@ -7502,7 +7502,7 @@
       <c r="Y49" s="11"/>
       <c r="Z49" s="20"/>
     </row>
-    <row r="50" spans="1:26" ht="174">
+    <row r="50" spans="1:26" ht="180">
       <c r="A50" s="12" t="s">
         <v>495</v>
       </c>
@@ -7560,7 +7560,7 @@
       <c r="Y50" s="11"/>
       <c r="Z50" s="12"/>
     </row>
-    <row r="51" spans="1:26" ht="174">
+    <row r="51" spans="1:26" ht="185.25">
       <c r="A51" s="12" t="s">
         <v>503</v>
       </c>
@@ -7616,7 +7616,7 @@
       <c r="Y51" s="11"/>
       <c r="Z51" s="20"/>
     </row>
-    <row r="52" spans="1:26" ht="126">
+    <row r="52" spans="1:26" ht="156.75">
       <c r="A52" s="12" t="s">
         <v>507</v>
       </c>
@@ -7823,13 +7823,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.81640625"/>
-    <col min="2" max="2" width="27.7265625"/>
-    <col min="3" max="3" width="31.26953125"/>
-    <col min="4" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="43.85546875"/>
+    <col min="2" max="2" width="27.7109375"/>
+    <col min="3" max="3" width="31.28515625"/>
+    <col min="4" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1">
@@ -8850,13 +8850,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.1796875"/>
-    <col min="2" max="2" width="34.7265625"/>
-    <col min="3" max="5" width="21.54296875"/>
-    <col min="6" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="27.140625"/>
+    <col min="2" max="2" width="34.7109375"/>
+    <col min="3" max="5" width="21.5703125"/>
+    <col min="6" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.75" customHeight="1">
@@ -9870,17 +9870,17 @@
   <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.81640625"/>
-    <col min="2" max="2" width="65.26953125"/>
-    <col min="3" max="3" width="12.26953125"/>
-    <col min="4" max="28" width="14.81640625"/>
-    <col min="29" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="25.85546875"/>
+    <col min="2" max="2" width="65.28515625"/>
+    <col min="3" max="3" width="12.28515625"/>
+    <col min="4" max="28" width="14.85546875"/>
+    <col min="29" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27.75" customHeight="1">
@@ -10593,12 +10593,12 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.26953125"/>
-    <col min="2" max="2" width="39.54296875"/>
-    <col min="3" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="24.28515625"/>
+    <col min="2" max="2" width="39.5703125"/>
+    <col min="3" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" customHeight="1">
@@ -11613,14 +11613,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.453125"/>
-    <col min="2" max="2" width="33.453125"/>
-    <col min="3" max="5" width="21.81640625"/>
+    <col min="1" max="1" width="26.42578125"/>
+    <col min="2" max="2" width="33.42578125"/>
+    <col min="3" max="5" width="21.85546875"/>
     <col min="6" max="6" width="26"/>
-    <col min="7" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="7" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27.75" customHeight="1">
@@ -11643,7 +11643,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="42">
+    <row r="2" spans="1:26" ht="42.75">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -11681,7 +11681,7 @@
       <c r="Y2" s="29"/>
       <c r="Z2" s="29"/>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="11" t="s">
         <v>49</v>
       </c>
@@ -11719,7 +11719,7 @@
       <c r="Y3" s="29"/>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" ht="72.5">
+    <row r="4" spans="1:26" ht="75">
       <c r="A4" s="11" t="s">
         <v>66</v>
       </c>
@@ -11757,7 +11757,7 @@
       <c r="Y4" s="29"/>
       <c r="Z4" s="29"/>
     </row>
-    <row r="5" spans="1:26" ht="42">
+    <row r="5" spans="1:26" ht="42.75">
       <c r="A5" s="11" t="s">
         <v>116</v>
       </c>
@@ -11795,7 +11795,7 @@
       <c r="Y5" s="29"/>
       <c r="Z5" s="29"/>
     </row>
-    <row r="6" spans="1:26" ht="87">
+    <row r="6" spans="1:26" ht="90">
       <c r="A6" s="11" t="s">
         <v>170</v>
       </c>
@@ -11833,7 +11833,7 @@
       <c r="Y6" s="29"/>
       <c r="Z6" s="29"/>
     </row>
-    <row r="7" spans="1:26" ht="56">
+    <row r="7" spans="1:26" ht="57">
       <c r="A7" s="12" t="s">
         <v>185</v>
       </c>
@@ -11871,7 +11871,7 @@
       <c r="Y7" s="29"/>
       <c r="Z7" s="29"/>
     </row>
-    <row r="8" spans="1:26" ht="42">
+    <row r="8" spans="1:26" ht="42.75">
       <c r="A8" s="12" t="s">
         <v>206</v>
       </c>
@@ -11909,7 +11909,7 @@
       <c r="Y8" s="29"/>
       <c r="Z8" s="29"/>
     </row>
-    <row r="9" spans="1:26" ht="72.5">
+    <row r="9" spans="1:26" ht="75">
       <c r="A9" s="12" t="s">
         <v>260</v>
       </c>
@@ -11927,7 +11927,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="98">
+    <row r="10" spans="1:26" ht="99.75">
       <c r="A10" s="11" t="s">
         <v>249</v>
       </c>
@@ -11965,7 +11965,7 @@
       <c r="Y10" s="29"/>
       <c r="Z10" s="29"/>
     </row>
-    <row r="11" spans="1:26" ht="42">
+    <row r="11" spans="1:26" ht="45">
       <c r="A11" s="12" t="s">
         <v>226</v>
       </c>
@@ -11983,7 +11983,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="58">
+    <row r="12" spans="1:26" ht="60">
       <c r="A12" s="12" t="s">
         <v>272</v>
       </c>
@@ -12001,7 +12001,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="58">
+    <row r="13" spans="1:26" ht="60">
       <c r="A13" s="11" t="s">
         <v>282</v>
       </c>
@@ -12019,7 +12019,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="70">
+    <row r="14" spans="1:26" ht="85.5">
       <c r="A14" s="12" t="s">
         <v>943</v>
       </c>
@@ -12037,7 +12037,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="70">
+    <row r="15" spans="1:26" ht="71.25">
       <c r="A15" s="12" t="s">
         <v>307</v>
       </c>
@@ -12055,7 +12055,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="56">
+    <row r="16" spans="1:26" ht="57">
       <c r="A16" s="12" t="s">
         <v>319</v>
       </c>
@@ -12073,7 +12073,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="42">
+    <row r="17" spans="1:6" ht="42.75">
       <c r="A17" s="12" t="s">
         <v>295</v>
       </c>
@@ -12091,7 +12091,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="70">
+    <row r="18" spans="1:6" ht="71.25">
       <c r="A18" s="12" t="s">
         <v>356</v>
       </c>
@@ -12109,7 +12109,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="70">
+    <row r="19" spans="1:6" ht="71.25">
       <c r="A19" s="12" t="s">
         <v>384</v>
       </c>
@@ -12127,7 +12127,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="42">
+    <row r="20" spans="1:6" ht="42.75">
       <c r="A20" s="12" t="s">
         <v>434</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="70">
+    <row r="21" spans="1:6" ht="71.25">
       <c r="A21" s="12" t="s">
         <v>446</v>
       </c>
@@ -12163,7 +12163,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="42">
+    <row r="22" spans="1:6" ht="42.75">
       <c r="A22" s="12" t="s">
         <v>498</v>
       </c>
@@ -12181,7 +12181,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="56">
+    <row r="23" spans="1:6" ht="57">
       <c r="A23" s="12" t="s">
         <v>481</v>
       </c>
@@ -12199,7 +12199,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="84">
+    <row r="24" spans="1:6" ht="85.5">
       <c r="A24" s="12" t="s">
         <v>489</v>
       </c>
@@ -13207,19 +13207,19 @@
   <dimension ref="A1:Y47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.453125"/>
-    <col min="2" max="2" width="50.7265625"/>
-    <col min="3" max="3" width="34.453125"/>
-    <col min="4" max="4" width="14.7265625"/>
-    <col min="5" max="25" width="14.81640625"/>
-    <col min="26" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="26.42578125"/>
+    <col min="2" max="2" width="50.7109375"/>
+    <col min="3" max="3" width="34.42578125"/>
+    <col min="4" max="4" width="14.7109375"/>
+    <col min="5" max="25" width="14.85546875"/>
+    <col min="26" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
@@ -13475,7 +13475,7 @@
       <c r="X17" s="29"/>
       <c r="Y17" s="29"/>
     </row>
-    <row r="18" spans="1:25" ht="42">
+    <row r="18" spans="1:25" ht="42.75">
       <c r="A18" s="31" t="s">
         <v>1015</v>
       </c>
@@ -13561,7 +13561,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" ht="29.25">
       <c r="A23" s="27" t="s">
         <v>1031</v>
       </c>
@@ -13868,15 +13868,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625"/>
-    <col min="2" max="26" width="8.54296875"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="10.85546875"/>
+    <col min="2" max="26" width="8.5703125"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14.25" customHeight="1">
@@ -13902,14 +13902,14 @@
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7265625"/>
-    <col min="2" max="2" width="34.453125"/>
-    <col min="3" max="3" width="19.1796875"/>
-    <col min="4" max="4" width="19.54296875"/>
-    <col min="5" max="26" width="14.81640625"/>
-    <col min="27" max="1024" width="14.1796875"/>
+    <col min="1" max="1" width="15.7109375"/>
+    <col min="2" max="2" width="34.42578125"/>
+    <col min="3" max="3" width="19.140625"/>
+    <col min="4" max="4" width="19.5703125"/>
+    <col min="5" max="26" width="14.85546875"/>
+    <col min="27" max="1024" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" customHeight="1">
@@ -14978,11 +14978,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.1796875"/>
-    <col min="2" max="27" width="8.54296875"/>
-    <col min="28" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="12.140625"/>
+    <col min="2" max="27" width="8.5703125"/>
+    <col min="28" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" customHeight="1">
@@ -16010,15 +16010,15 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.81640625"/>
-    <col min="2" max="2" width="27.7265625"/>
-    <col min="3" max="3" width="31.26953125"/>
-    <col min="4" max="4" width="21.26953125"/>
-    <col min="5" max="5" width="14.453125"/>
-    <col min="6" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="43.85546875"/>
+    <col min="2" max="2" width="27.7109375"/>
+    <col min="3" max="3" width="31.28515625"/>
+    <col min="4" max="4" width="21.28515625"/>
+    <col min="5" max="5" width="14.42578125"/>
+    <col min="6" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
@@ -16038,7 +16038,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="58">
+    <row r="2" spans="1:7" ht="60">
       <c r="A2" s="12" t="s">
         <v>513</v>
       </c>
@@ -16054,7 +16054,7 @@
       <c r="E2" s="25"/>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="1:7" ht="58">
+    <row r="3" spans="1:7" ht="60">
       <c r="A3" s="11" t="s">
         <v>517</v>
       </c>
@@ -16070,7 +16070,7 @@
       <c r="E3" s="25"/>
       <c r="G3" s="29"/>
     </row>
-    <row r="4" spans="1:7" ht="29">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="11" t="s">
         <v>521</v>
       </c>
@@ -16086,7 +16086,7 @@
       <c r="E4" s="25"/>
       <c r="G4" s="29"/>
     </row>
-    <row r="5" spans="1:7" ht="29">
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="11" t="s">
         <v>134</v>
       </c>
@@ -16102,7 +16102,7 @@
       <c r="E5" s="25"/>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" ht="29">
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="11" t="s">
         <v>527</v>
       </c>
@@ -16118,7 +16118,7 @@
       <c r="E6" s="25"/>
       <c r="G6" s="29"/>
     </row>
-    <row r="7" spans="1:7" ht="58">
+    <row r="7" spans="1:7" ht="60">
       <c r="A7" s="11" t="s">
         <v>529</v>
       </c>
@@ -16134,7 +16134,7 @@
       <c r="E7" s="25"/>
       <c r="G7" s="29"/>
     </row>
-    <row r="8" spans="1:7" ht="43.5">
+    <row r="8" spans="1:7" ht="60">
       <c r="A8" s="11" t="s">
         <v>532</v>
       </c>
@@ -16150,7 +16150,7 @@
       <c r="E8" s="25"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" ht="29">
+    <row r="9" spans="1:7" ht="45">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -16166,7 +16166,7 @@
       <c r="E9" s="25"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" ht="58">
+    <row r="10" spans="1:7" ht="60">
       <c r="A10" s="11" t="s">
         <v>539</v>
       </c>
@@ -17178,15 +17178,15 @@
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.81640625"/>
-    <col min="2" max="2" width="27.7265625"/>
-    <col min="3" max="3" width="31.26953125"/>
-    <col min="4" max="4" width="21.26953125"/>
-    <col min="5" max="5" width="14.453125"/>
-    <col min="6" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="43.85546875"/>
+    <col min="2" max="2" width="27.7109375"/>
+    <col min="3" max="3" width="31.28515625"/>
+    <col min="4" max="4" width="21.28515625"/>
+    <col min="5" max="5" width="14.42578125"/>
+    <col min="6" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1">
@@ -17227,7 +17227,7 @@
       <c r="Y1" s="25"/>
       <c r="Z1" s="25"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" s="11" t="s">
         <v>416</v>
       </c>
@@ -17263,7 +17263,7 @@
       <c r="Y2" s="31"/>
       <c r="Z2" s="31"/>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="11" t="s">
         <v>545</v>
       </c>
@@ -17299,7 +17299,7 @@
       <c r="Y3" s="31"/>
       <c r="Z3" s="31"/>
     </row>
-    <row r="4" spans="1:26" ht="43.5">
+    <row r="4" spans="1:26" ht="45">
       <c r="A4" s="11" t="s">
         <v>286</v>
       </c>
@@ -17335,7 +17335,7 @@
       <c r="Y4" s="31"/>
       <c r="Z4" s="31"/>
     </row>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" s="11" t="s">
         <v>162</v>
       </c>
@@ -17371,7 +17371,7 @@
       <c r="Y5" s="31"/>
       <c r="Z5" s="31"/>
     </row>
-    <row r="6" spans="1:26" ht="29">
+    <row r="6" spans="1:26" ht="30">
       <c r="A6" s="11" t="s">
         <v>360</v>
       </c>
@@ -17407,7 +17407,7 @@
       <c r="Y6" s="31"/>
       <c r="Z6" s="31"/>
     </row>
-    <row r="7" spans="1:26" ht="29">
+    <row r="7" spans="1:26" ht="30">
       <c r="A7" s="11" t="s">
         <v>556</v>
       </c>
@@ -17443,7 +17443,7 @@
       <c r="Y7" s="31"/>
       <c r="Z7" s="31"/>
     </row>
-    <row r="8" spans="1:26" ht="43.5">
+    <row r="8" spans="1:26" ht="60">
       <c r="A8" s="11" t="s">
         <v>559</v>
       </c>
@@ -17479,7 +17479,7 @@
       <c r="Y8" s="31"/>
       <c r="Z8" s="31"/>
     </row>
-    <row r="9" spans="1:26" ht="43.5">
+    <row r="9" spans="1:26" ht="60">
       <c r="A9" s="11" t="s">
         <v>265</v>
       </c>
@@ -17515,7 +17515,7 @@
       <c r="Y9" s="31"/>
       <c r="Z9" s="31"/>
     </row>
-    <row r="10" spans="1:26" ht="29">
+    <row r="10" spans="1:26" ht="30">
       <c r="A10" s="11" t="s">
         <v>564</v>
       </c>
@@ -17551,7 +17551,7 @@
       <c r="Y10" s="31"/>
       <c r="Z10" s="31"/>
     </row>
-    <row r="11" spans="1:26" ht="29">
+    <row r="11" spans="1:26" ht="30">
       <c r="A11" s="11" t="s">
         <v>493</v>
       </c>
@@ -18579,18 +18579,18 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="20.7265625"/>
-    <col min="3" max="3" width="34.54296875"/>
-    <col min="4" max="4" width="53.1796875"/>
-    <col min="5" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="1" max="2" width="20.7109375"/>
+    <col min="3" max="3" width="34.5703125"/>
+    <col min="4" max="4" width="53.140625"/>
+    <col min="5" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="25.5" customHeight="1">
@@ -19646,13 +19646,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.81640625"/>
-    <col min="2" max="2" width="31.26953125"/>
-    <col min="3" max="3" width="27.7265625"/>
-    <col min="4" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="43.85546875"/>
+    <col min="2" max="2" width="31.28515625"/>
+    <col min="3" max="3" width="27.7109375"/>
+    <col min="4" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1">
@@ -20706,13 +20706,13 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.81640625"/>
-    <col min="2" max="2" width="126.26953125"/>
-    <col min="3" max="3" width="27.7265625"/>
-    <col min="4" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="43.85546875"/>
+    <col min="2" max="2" width="126.28515625"/>
+    <col min="3" max="3" width="27.7109375"/>
+    <col min="4" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1">
@@ -20749,7 +20749,7 @@
       <c r="Y1" s="25"/>
       <c r="Z1" s="25"/>
     </row>
-    <row r="2" spans="1:26" ht="391.5">
+    <row r="2" spans="1:26" ht="409.5">
       <c r="A2" s="11" t="s">
         <v>56</v>
       </c>
@@ -20813,7 +20813,7 @@
       <c r="Y3" s="25"/>
       <c r="Z3" s="25"/>
     </row>
-    <row r="4" spans="1:26" ht="29">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" s="11" t="s">
         <v>96</v>
       </c>
@@ -20845,7 +20845,7 @@
       <c r="Y4" s="25"/>
       <c r="Z4" s="25"/>
     </row>
-    <row r="5" spans="1:26" ht="101.5">
+    <row r="5" spans="1:26" ht="105">
       <c r="A5" s="11" t="s">
         <v>104</v>
       </c>
@@ -20877,7 +20877,7 @@
       <c r="Y5" s="25"/>
       <c r="Z5" s="25"/>
     </row>
-    <row r="6" spans="1:26" ht="101.5">
+    <row r="6" spans="1:26" ht="105">
       <c r="A6" s="11" t="s">
         <v>110</v>
       </c>
@@ -20909,7 +20909,7 @@
       <c r="Y6" s="25"/>
       <c r="Z6" s="25"/>
     </row>
-    <row r="7" spans="1:26" ht="29">
+    <row r="7" spans="1:26" ht="30">
       <c r="A7" s="11" t="s">
         <v>136</v>
       </c>
@@ -20941,7 +20941,7 @@
       <c r="Y7" s="25"/>
       <c r="Z7" s="25"/>
     </row>
-    <row r="8" spans="1:26" ht="145">
+    <row r="8" spans="1:26" ht="150">
       <c r="A8" s="11" t="s">
         <v>146</v>
       </c>
@@ -20973,7 +20973,7 @@
       <c r="Y8" s="25"/>
       <c r="Z8" s="25"/>
     </row>
-    <row r="9" spans="1:26" ht="188.5">
+    <row r="9" spans="1:26" ht="195">
       <c r="A9" s="11" t="s">
         <v>164</v>
       </c>
@@ -21005,7 +21005,7 @@
       <c r="Y9" s="25"/>
       <c r="Z9" s="25"/>
     </row>
-    <row r="10" spans="1:26" ht="217.5">
+    <row r="10" spans="1:26" ht="225">
       <c r="A10" s="11" t="s">
         <v>177</v>
       </c>
@@ -21037,7 +21037,7 @@
       <c r="Y10" s="25"/>
       <c r="Z10" s="25"/>
     </row>
-    <row r="11" spans="1:26" ht="130.5">
+    <row r="11" spans="1:26" ht="135">
       <c r="A11" s="11" t="s">
         <v>211</v>
       </c>
@@ -21069,7 +21069,7 @@
       <c r="Y11" s="25"/>
       <c r="Z11" s="25"/>
     </row>
-    <row r="12" spans="1:26" ht="29">
+    <row r="12" spans="1:26" ht="30">
       <c r="A12" s="11" t="s">
         <v>220</v>
       </c>
@@ -21133,7 +21133,7 @@
       <c r="Y13" s="25"/>
       <c r="Z13" s="25"/>
     </row>
-    <row r="14" spans="1:26" ht="72.5">
+    <row r="14" spans="1:26" ht="90">
       <c r="A14" s="11" t="s">
         <v>287</v>
       </c>
@@ -21197,7 +21197,7 @@
       <c r="Y15" s="25"/>
       <c r="Z15" s="25"/>
     </row>
-    <row r="16" spans="1:26" ht="84">
+    <row r="16" spans="1:26" ht="85.5">
       <c r="A16" s="11" t="s">
         <v>337</v>
       </c>
@@ -21293,7 +21293,7 @@
       <c r="Y18" s="25"/>
       <c r="Z18" s="25"/>
     </row>
-    <row r="19" spans="1:26" ht="87">
+    <row r="19" spans="1:26" ht="90">
       <c r="A19" s="11" t="s">
         <v>370</v>
       </c>
@@ -22399,15 +22399,15 @@
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.26953125"/>
-    <col min="2" max="2" width="78.7265625"/>
-    <col min="3" max="3" width="50.26953125"/>
-    <col min="4" max="4" width="21.54296875"/>
-    <col min="5" max="5" width="36.453125"/>
-    <col min="6" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="1" max="1" width="55.28515625"/>
+    <col min="2" max="2" width="78.7109375"/>
+    <col min="3" max="3" width="50.28515625"/>
+    <col min="4" max="4" width="21.5703125"/>
+    <col min="5" max="5" width="36.42578125"/>
+    <col min="6" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1">
@@ -22438,7 +22438,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28">
+    <row r="3" spans="1:6" ht="28.5">
       <c r="A3" s="12" t="s">
         <v>601</v>
       </c>
@@ -22446,7 +22446,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="84">
+    <row r="4" spans="1:6" ht="85.5">
       <c r="A4" s="12" t="s">
         <v>603</v>
       </c>
@@ -22454,7 +22454,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="70">
+    <row r="5" spans="1:6" ht="71.25">
       <c r="A5" s="12" t="s">
         <v>57</v>
       </c>
@@ -22462,7 +22462,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28">
+    <row r="6" spans="1:6" ht="28.5">
       <c r="A6" s="12" t="s">
         <v>606</v>
       </c>
@@ -22478,7 +22478,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28">
+    <row r="8" spans="1:6" ht="28.5">
       <c r="A8" s="12" t="s">
         <v>610</v>
       </c>
@@ -22486,7 +22486,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="28.5">
       <c r="A9" s="12" t="s">
         <v>612</v>
       </c>
@@ -22497,7 +22497,7 @@
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:6" ht="28">
+    <row r="10" spans="1:6" ht="28.5">
       <c r="A10" s="12" t="s">
         <v>614</v>
       </c>
@@ -22508,7 +22508,7 @@
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:6" ht="28">
+    <row r="11" spans="1:6" ht="28.5">
       <c r="A11" s="12" t="s">
         <v>616</v>
       </c>
@@ -22527,7 +22527,7 @@
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:6" ht="84">
+    <row r="13" spans="1:6" ht="85.5">
       <c r="A13" s="12" t="s">
         <v>620</v>
       </c>
@@ -22538,7 +22538,7 @@
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:6" ht="28">
+    <row r="14" spans="1:6" ht="28.5">
       <c r="A14" s="15" t="s">
         <v>621</v>
       </c>
@@ -22549,7 +22549,7 @@
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="28.5">
       <c r="A15" s="15" t="s">
         <v>623</v>
       </c>
@@ -22560,7 +22560,7 @@
       <c r="D15" s="25"/>
       <c r="E15" s="33"/>
     </row>
-    <row r="16" spans="1:6" ht="56">
+    <row r="16" spans="1:6" ht="57">
       <c r="A16" s="15" t="s">
         <v>625</v>
       </c>
@@ -22571,7 +22571,7 @@
       <c r="D16" s="25"/>
       <c r="E16" s="33"/>
     </row>
-    <row r="17" spans="1:5" ht="28">
+    <row r="17" spans="1:5" ht="28.5">
       <c r="A17" s="15" t="s">
         <v>627</v>
       </c>
@@ -22582,7 +22582,7 @@
       <c r="D17" s="25"/>
       <c r="E17" s="33"/>
     </row>
-    <row r="18" spans="1:5" ht="42">
+    <row r="18" spans="1:5" ht="57">
       <c r="A18" s="15" t="s">
         <v>629</v>
       </c>
@@ -22593,7 +22593,7 @@
       <c r="D18" s="25"/>
       <c r="E18" s="33"/>
     </row>
-    <row r="19" spans="1:5" ht="28">
+    <row r="19" spans="1:5" ht="28.5">
       <c r="A19" s="15" t="s">
         <v>631</v>
       </c>
@@ -22604,7 +22604,7 @@
       <c r="D19" s="25"/>
       <c r="E19" s="33"/>
     </row>
-    <row r="20" spans="1:5" ht="42">
+    <row r="20" spans="1:5" ht="57">
       <c r="A20" s="15" t="s">
         <v>633</v>
       </c>
@@ -22615,7 +22615,7 @@
       <c r="D20" s="25"/>
       <c r="E20" s="33"/>
     </row>
-    <row r="21" spans="1:5" ht="28">
+    <row r="21" spans="1:5" ht="28.5">
       <c r="A21" s="15" t="s">
         <v>635</v>
       </c>
@@ -22648,7 +22648,7 @@
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
     </row>
-    <row r="24" spans="1:5" ht="42">
+    <row r="24" spans="1:5" ht="42.75">
       <c r="A24" s="12" t="s">
         <v>641</v>
       </c>
@@ -22659,7 +22659,7 @@
       <c r="D24" s="25"/>
       <c r="E24" s="25"/>
     </row>
-    <row r="25" spans="1:5" ht="56">
+    <row r="25" spans="1:5" ht="57">
       <c r="A25" s="12" t="s">
         <v>137</v>
       </c>
@@ -22670,7 +22670,7 @@
       <c r="D25" s="25"/>
       <c r="E25" s="25"/>
     </row>
-    <row r="26" spans="1:5" ht="28">
+    <row r="26" spans="1:5" ht="28.5">
       <c r="A26" s="12" t="s">
         <v>644</v>
       </c>
@@ -22747,7 +22747,7 @@
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
     </row>
-    <row r="33" spans="1:5" ht="28">
+    <row r="33" spans="1:5" ht="28.5">
       <c r="A33" s="12" t="s">
         <v>657</v>
       </c>
@@ -22769,7 +22769,7 @@
       <c r="D34" s="25"/>
       <c r="E34" s="25"/>
     </row>
-    <row r="35" spans="1:5" ht="56">
+    <row r="35" spans="1:5" ht="57">
       <c r="A35" s="12" t="s">
         <v>198</v>
       </c>
@@ -22780,7 +22780,7 @@
       <c r="D35" s="25"/>
       <c r="E35" s="25"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" ht="28.5">
       <c r="A36" s="12" t="s">
         <v>661</v>
       </c>
@@ -22835,7 +22835,7 @@
       <c r="D40" s="25"/>
       <c r="E40" s="25"/>
     </row>
-    <row r="41" spans="1:5" ht="28">
+    <row r="41" spans="1:5" ht="28.5">
       <c r="A41" s="12" t="s">
         <v>671</v>
       </c>
@@ -22890,7 +22890,7 @@
       <c r="D45" s="25"/>
       <c r="E45" s="25"/>
     </row>
-    <row r="46" spans="1:5" ht="42">
+    <row r="46" spans="1:5" ht="42.75">
       <c r="A46" s="12" t="s">
         <v>680</v>
       </c>
@@ -22901,7 +22901,7 @@
       <c r="D46" s="25"/>
       <c r="E46" s="25"/>
     </row>
-    <row r="47" spans="1:5" ht="42">
+    <row r="47" spans="1:5" ht="42.75">
       <c r="A47" s="12" t="s">
         <v>682</v>
       </c>
@@ -22945,7 +22945,7 @@
       <c r="D50" s="25"/>
       <c r="E50" s="25"/>
     </row>
-    <row r="51" spans="1:5" ht="56">
+    <row r="51" spans="1:5" ht="71.25">
       <c r="A51" s="12" t="s">
         <v>243</v>
       </c>
@@ -22967,7 +22967,7 @@
       <c r="D52" s="25"/>
       <c r="E52" s="25"/>
     </row>
-    <row r="53" spans="1:5" ht="28">
+    <row r="53" spans="1:5" ht="28.5">
       <c r="A53" s="12" t="s">
         <v>693</v>
       </c>
@@ -22989,7 +22989,7 @@
       <c r="D54" s="25"/>
       <c r="E54" s="25"/>
     </row>
-    <row r="55" spans="1:5" ht="28">
+    <row r="55" spans="1:5" ht="28.5">
       <c r="A55" s="12" t="s">
         <v>697</v>
       </c>
@@ -23019,7 +23019,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="42">
+    <row r="58" spans="1:5" ht="42.75">
       <c r="A58" s="12" t="s">
         <v>311</v>
       </c>
@@ -23043,7 +23043,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="28">
+    <row r="61" spans="1:5" ht="28.5">
       <c r="A61" s="12" t="s">
         <v>705</v>
       </c>
@@ -23059,7 +23059,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="56">
+    <row r="63" spans="1:5" ht="71.25">
       <c r="A63" s="12" t="s">
         <v>708</v>
       </c>
@@ -23091,7 +23091,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="28">
+    <row r="67" spans="1:2" ht="28.5">
       <c r="A67" s="12" t="s">
         <v>442</v>
       </c>
@@ -23121,20 +23121,20 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.26953125"/>
-    <col min="2" max="2" width="10.26953125"/>
-    <col min="3" max="3" width="14.81640625"/>
+    <col min="1" max="1" width="40.28515625"/>
+    <col min="2" max="2" width="10.28515625"/>
+    <col min="3" max="3" width="14.85546875"/>
     <col min="4" max="4" width="49"/>
-    <col min="5" max="5" width="14.81640625"/>
-    <col min="6" max="6" width="18.54296875"/>
-    <col min="7" max="26" width="14.81640625"/>
-    <col min="27" max="1025" width="14.1796875"/>
+    <col min="5" max="5" width="14.85546875"/>
+    <col min="6" max="6" width="18.5703125"/>
+    <col min="7" max="26" width="14.85546875"/>
+    <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1">
@@ -23179,7 +23179,7 @@
       </c>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:6" ht="58">
+    <row r="4" spans="1:6" ht="75">
       <c r="A4" s="15" t="s">
         <v>722</v>
       </c>
@@ -23190,7 +23190,7 @@
       </c>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:6" ht="203">
+    <row r="5" spans="1:6" ht="240">
       <c r="A5" s="15" t="s">
         <v>245</v>
       </c>
@@ -23201,7 +23201,7 @@
       </c>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:6" ht="112">
+    <row r="6" spans="1:6" ht="114">
       <c r="A6" s="15" t="s">
         <v>725</v>
       </c>
@@ -23211,7 +23211,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28">
+    <row r="7" spans="1:6" ht="28.5">
       <c r="A7" s="15" t="s">
         <v>363</v>
       </c>
@@ -23221,7 +23221,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="42">
+    <row r="8" spans="1:6" ht="42.75">
       <c r="A8" s="15" t="s">
         <v>373</v>
       </c>
@@ -24228,14 +24228,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="45"/>
-    <col min="2" max="2" width="82.54296875"/>
-    <col min="3" max="6" width="14.81640625"/>
-    <col min="7" max="7" width="21.1796875"/>
-    <col min="8" max="27" width="14.81640625"/>
-    <col min="28" max="1025" width="14.1796875"/>
+    <col min="2" max="2" width="82.5703125"/>
+    <col min="3" max="6" width="14.85546875"/>
+    <col min="7" max="7" width="21.140625"/>
+    <col min="8" max="27" width="14.85546875"/>
+    <col min="28" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1">
@@ -24261,7 +24261,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="154.5">
+    <row r="2" spans="1:7" ht="171.75">
       <c r="A2" s="32" t="s">
         <v>61</v>
       </c>
@@ -24271,7 +24271,7 @@
       <c r="C2" s="38"/>
       <c r="D2" s="38"/>
     </row>
-    <row r="3" spans="1:7" ht="168.5">
+    <row r="3" spans="1:7" ht="186">
       <c r="A3" s="32" t="s">
         <v>125</v>
       </c>
@@ -24279,7 +24279,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="182.5">
+    <row r="4" spans="1:7" ht="186">
       <c r="A4" s="32" t="s">
         <v>215</v>
       </c>
@@ -24287,7 +24287,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="168.5">
+    <row r="5" spans="1:7" ht="186">
       <c r="A5" s="32" t="s">
         <v>43</v>
       </c>
@@ -24297,7 +24297,7 @@
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
     </row>
-    <row r="6" spans="1:7" ht="87">
+    <row r="6" spans="1:7" ht="105">
       <c r="A6" s="32" t="s">
         <v>77</v>
       </c>
@@ -24308,7 +24308,7 @@
       <c r="D6" s="38"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:7" ht="56.5">
+    <row r="7" spans="1:7" ht="57.75">
       <c r="A7" s="32" t="s">
         <v>411</v>
       </c>
@@ -24316,7 +24316,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.5">
+    <row r="8" spans="1:7" ht="29.25">
       <c r="A8" s="32" t="s">
         <v>166</v>
       </c>
@@ -24324,7 +24324,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="84.5">
+    <row r="9" spans="1:7" ht="86.25">
       <c r="A9" s="32" t="s">
         <v>181</v>
       </c>
@@ -24332,7 +24332,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="56.5">
+    <row r="10" spans="1:7" ht="57.75">
       <c r="A10" s="32" t="s">
         <v>256</v>
       </c>
@@ -24340,7 +24340,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="70.5">
+    <row r="11" spans="1:7" ht="72">
       <c r="A11" s="32" t="s">
         <v>314</v>
       </c>
@@ -24348,7 +24348,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="140.5">
+    <row r="12" spans="1:7" ht="143.25">
       <c r="A12" s="26" t="s">
         <v>278</v>
       </c>
@@ -24356,7 +24356,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="126.5">
+    <row r="13" spans="1:7" ht="129">
       <c r="A13" s="32" t="s">
         <v>291</v>
       </c>
@@ -24364,7 +24364,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="70.5">
+    <row r="14" spans="1:7" ht="72">
       <c r="A14" s="32" t="s">
         <v>303</v>
       </c>
@@ -24372,7 +24372,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="238.5">
+    <row r="15" spans="1:7" ht="243">
       <c r="A15" s="32" t="s">
         <v>201</v>
       </c>
@@ -24380,7 +24380,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="308.5">
+    <row r="16" spans="1:7" ht="342.75">
       <c r="A16" s="32" t="s">
         <v>237</v>
       </c>

</xml_diff>